<commit_message>
ver 0.2 2020/08/16 [320304/28124] - 3 water sensor added
</commit_message>
<xml_diff>
--- a/WaterSupplyControl_web/WaterSupplyControl.xlsx
+++ b/WaterSupplyControl_web/WaterSupplyControl.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WaterSupplyControl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WaterSupplyControl_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F170343F-3FC5-4070-9652-38328A225ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2540981B-09BF-45AB-9B54-CB2A65D3A3CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{48510476-7EAF-4049-AE02-C36CE8CD78F1}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
   <si>
     <t>Contactless water sensor</t>
   </si>
@@ -288,6 +288,54 @@
   </si>
   <si>
     <t>3V</t>
+  </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>relay H2_2</t>
+  </si>
+  <si>
+    <t>relay H2_1</t>
+  </si>
+  <si>
+    <t>relay H1_1</t>
+  </si>
+  <si>
+    <t>led</t>
+  </si>
+  <si>
+    <t>no int</t>
+  </si>
+  <si>
+    <t>low at start</t>
+  </si>
+  <si>
+    <t>занят при загрузке</t>
+  </si>
+  <si>
+    <t>relay H1_2</t>
+  </si>
+  <si>
+    <t>relay H3_2</t>
+  </si>
+  <si>
+    <t>relay H3_1</t>
+  </si>
+  <si>
+    <t>Wsens 1</t>
+  </si>
+  <si>
+    <t>Wsens 2</t>
+  </si>
+  <si>
+    <t>Wsen не получается, всегда 1; relay - на старте всегда Low. Как его использовать?!</t>
+  </si>
+  <si>
+    <t>Wsens 3</t>
   </si>
 </sst>
 </file>
@@ -361,8 +409,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF7030A0"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -370,7 +417,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -378,7 +424,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.249977111117893"/>
+      <color theme="1" tint="0.34998626667073579"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -386,14 +432,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,6 +458,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -425,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -441,10 +511,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -467,13 +540,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
@@ -534,15 +607,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -572,7 +645,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="247650" y="2032000"/>
+          <a:off x="190500" y="2057400"/>
           <a:ext cx="6877050" cy="4819650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -953,112 +1026,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C6101F-AAA7-461F-8460-D35B041821C2}">
-  <dimension ref="A3:E22"/>
+  <dimension ref="A3:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>70</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>71</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>75</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>73</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>76</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>81</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D22" s="6">
-        <f>COUNTA(D2:D19)</f>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="E22" s="6">
+        <f>COUNTA(E2:E19)</f>
         <v>10</v>
       </c>
     </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="E28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>94</v>
+      </c>
+      <c r="G30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32">
+        <v>14</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34">
+        <v>13</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E35" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E38" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E40" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E41" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E42" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E43" s="13"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1067,7 +1283,7 @@
   <dimension ref="A1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1128,10 +1344,10 @@
       <c r="C39" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="D39" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="G39" t="s">
+      <c r="E39" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1142,7 +1358,7 @@
       <c r="C40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="D40" s="16" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1150,10 +1366,10 @@
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="D41" s="15" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1161,10 +1377,10 @@
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="14" t="s">
+      <c r="C42" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="D42" s="14" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ver 0.5 2020/08/16 [322776/28536] - fully working device with: 2 relays, 3 water level sensors and waterflow sensor
</commit_message>
<xml_diff>
--- a/WaterSupplyControl_web/WaterSupplyControl.xlsx
+++ b/WaterSupplyControl_web/WaterSupplyControl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WaterSupplyControl_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2540981B-09BF-45AB-9B54-CB2A65D3A3CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E212BBEF-AB7E-4DCF-9BDF-2CF6F1E306F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{48510476-7EAF-4049-AE02-C36CE8CD78F1}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="106">
   <si>
     <t>Contactless water sensor</t>
   </si>
@@ -336,13 +336,22 @@
   </si>
   <si>
     <t>Wsens 3</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                                                                                                                                                                                                                                                                              </t>
+  </si>
+  <si>
+    <t>Wflow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,14 +410,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="7" tint="0.59999389629810485"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -438,8 +439,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -482,6 +499,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -495,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -508,17 +543,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1029,7 +1067,7 @@
   <dimension ref="A3:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection activeCell="E37" sqref="E37:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1177,7 @@
       <c r="C27" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="E27" s="9" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1175,6 +1213,9 @@
       <c r="C30" t="s">
         <v>94</v>
       </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
       <c r="G30" t="s">
         <v>101</v>
       </c>
@@ -1197,7 +1238,7 @@
       <c r="B32">
         <v>14</v>
       </c>
-      <c r="E32" s="12" t="s">
+      <c r="E32" s="9" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1208,7 +1249,7 @@
       <c r="B33">
         <v>12</v>
       </c>
-      <c r="E33" s="12" t="s">
+      <c r="E33" s="9" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1219,7 +1260,7 @@
       <c r="B34">
         <v>13</v>
       </c>
-      <c r="E34" s="12" t="s">
+      <c r="E34" s="9" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1237,41 +1278,24 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E37" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E39" t="s">
-        <v>17</v>
-      </c>
-    </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E40" s="13" t="s">
-        <v>21</v>
-      </c>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="10" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="10" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E43" s="13"/>
+      <c r="E43" s="10"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -1344,7 +1368,7 @@
       <c r="C39" t="s">
         <v>13</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="14" t="s">
         <v>12</v>
       </c>
       <c r="E39" t="s">
@@ -1358,7 +1382,7 @@
       <c r="C40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1366,10 +1390,10 @@
       <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="12" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1377,10 +1401,10 @@
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D42" s="14" t="s">
+      <c r="D42" s="11" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1397,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8F8D08-EB2F-4FE7-8856-D5C79DC74A6F}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1409,51 +1433,60 @@
     <col min="2" max="2" width="33.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="G3" s="8" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="G3" s="18" t="s">
         <v>66</v>
       </c>
       <c r="H3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I3" s="21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H4" t="s">
         <v>67</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="K4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="16" t="s">
         <v>1</v>
       </c>
       <c r="H5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I5" s="19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
@@ -1461,7 +1494,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1469,7 +1502,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1477,7 +1510,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>34</v>
       </c>
@@ -1485,7 +1518,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>36</v>
       </c>
@@ -1493,7 +1526,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>38</v>
       </c>
@@ -1501,15 +1534,18 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>42</v>
       </c>
@@ -1517,7 +1553,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
@@ -1525,7 +1561,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>46</v>
       </c>
@@ -1533,7 +1569,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
[WaterSupply] ver 0.6 2020/10/23 [343236/29368] - OTA added
</commit_message>
<xml_diff>
--- a/WaterSupplyControl_web/WaterSupplyControl.xlsx
+++ b/WaterSupplyControl_web/WaterSupplyControl.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WaterSupplyControl_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E212BBEF-AB7E-4DCF-9BDF-2CF6F1E306F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7DC45B-7D78-4BE0-9561-136A2CC44EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{48510476-7EAF-4049-AE02-C36CE8CD78F1}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="WaterFLow" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>

<commit_message>
[WaterSupply] ver 0.8d2020/10/30 [345932/31724] - web debug info improvents
</commit_message>
<xml_diff>
--- a/WaterSupplyControl_web/WaterSupplyControl.xlsx
+++ b/WaterSupplyControl_web/WaterSupplyControl.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emchenko\Documents\Arduino\WaterSupplyControl_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521FC1E4-80DB-4C48-A0D1-511F0EF9FFA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B5FFDB-39A4-490F-A7F3-0F977018D09F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{48510476-7EAF-4049-AE02-C36CE8CD78F1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="2" xr2:uid="{48510476-7EAF-4049-AE02-C36CE8CD78F1}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="2" r:id="rId1"/>
     <sheet name="Схема" sheetId="4" r:id="rId2"/>
-    <sheet name="water sensor" sheetId="1" r:id="rId3"/>
-    <sheet name="WaterFLow" sheetId="3" r:id="rId4"/>
+    <sheet name="Двигатель" sheetId="5" r:id="rId3"/>
+    <sheet name="water sensor" sheetId="1" r:id="rId4"/>
+    <sheet name="WaterFLow" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="109">
   <si>
     <t>Contactless water sensor</t>
   </si>
@@ -346,6 +347,15 @@
   </si>
   <si>
     <t>Wflow</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -543,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -572,6 +582,9 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -580,6 +593,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4472C4"/>
+      <color rgb="FFFFFFFF"/>
       <color rgb="FFE7E6E6"/>
       <color rgb="FF225686"/>
     </mruColors>
@@ -3384,14 +3399,14 @@
     <xdr:from>
       <xdr:col>34</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>169862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -3406,7 +3421,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8035925" y="3305175"/>
+          <a:off x="8035925" y="3273425"/>
           <a:ext cx="690563" cy="133350"/>
           <a:chOff x="6400800" y="3251200"/>
           <a:chExt cx="685800" cy="133350"/>
@@ -6951,6 +6966,2243 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D5152D-2551-4CD3-95A2-3C2D0E4F0332}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="818745" y="734979"/>
+          <a:ext cx="2456234" cy="1102468"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:alpha val="50196"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>148616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>32425</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Блок-схема: узел 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{339C2014-4F27-4ED6-895F-468B7D3BEECF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1052758" y="883595"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1631</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>151318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>72958</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>40027</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Блок-схема: узел 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F1C0CDE-356F-4467-B5C7-824F2EE08D11}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1639120" y="886297"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>151318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>32425</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>40027</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Блок-схема: узел 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A6A0F5E-369E-4FD5-B8CD-BD391C3D1506}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2963162" y="886297"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>32425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Блок-схема: узел 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42F6789C-942E-4650-9D25-0E25F8511F6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1052758" y="1618574"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>269142</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>67554</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Блок-схема: узел 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11107274-3920-4DCB-9D4C-BD053B893434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1633716" y="1618574"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>234014</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>32426</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Блок-схема: узел 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E5AE071-F610-4A19-8BEA-851741F23349}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2690248" y="1618574"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>32425</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Блок-схема: узел 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F610BB60-843B-4B02-ADEE-A39BD62ED42A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2963162" y="1618574"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193481</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>151318</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>264808</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>40027</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Блок-схема: узел 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA9437FB-4E0E-4169-8533-69FF8C07BC4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1830970" y="886297"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>32426</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Блок-схема: узел 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFB09165-A690-49AB-88D2-4EEDDBF91ACA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1325673" y="1618574"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193481</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>264808</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Блок-схема: узел 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88989BB5-1C5C-4AC2-B79D-3B48293710E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1830970" y="1618574"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>186446</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>27021</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>186447</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>27021</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Овал 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7014770F-E446-49CC-8E65-BEDE466AA3A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1005191" y="210766"/>
+          <a:ext cx="1091660" cy="1102468"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="4472C4">
+            <a:alpha val="50196"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>234014</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>151319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>32426</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>40027</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Блок-схема: узел 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFB72C5-6380-47B0-916A-D8A0D89C59E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1598588" y="1070042"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>234014</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>159424</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>32426</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>48133</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Блок-схема: узел 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27A2ED3-790F-4FB0-B953-FFB544142220}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1598588" y="343169"/>
+          <a:ext cx="71327" cy="72453"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>37295</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>151318</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="20" name="Прямая со стрелкой 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13809B2-99AB-4016-B7EA-76366061D641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1637490" y="1102468"/>
+          <a:ext cx="37294" cy="886297"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="oval"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>72958</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193481</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>3801</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Прямая со стрелкой 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491412E0-842B-403D-8157-CCF870ECEE03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="14" idx="2"/>
+          <a:endCxn id="5" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1710447" y="2024992"/>
+          <a:ext cx="120523" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>31891</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>148617</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Прямая со стрелкой 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9BEBB12-7ECA-4C8C-8B58-2A01DB2D0111}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="10" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1669380" y="1102468"/>
+          <a:ext cx="1059769" cy="1618575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575" cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="arrow"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Прямая со стрелкой 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39EC620D-7AAB-4032-BF4D-FD333A71B281}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2729149" y="1102469"/>
+          <a:ext cx="545830" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575" cmpd="dbl">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>5404</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>183744</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>183744</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Прямая со стрелкой 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D89A8339-7F32-43BE-9FF8-4E7C1C4C0230}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1642893" y="367489"/>
+          <a:ext cx="1632086" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>254001</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>118893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>35129</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>68499</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="35" name="Группа 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5920F2EF-6164-4681-BE9E-FF2F9A73A6ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1072746" y="1956340"/>
+          <a:ext cx="599872" cy="133350"/>
+          <a:chOff x="6400800" y="3251200"/>
+          <a:chExt cx="685800" cy="133350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="36" name="Прямая соединительная линия 35">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC6D38A5-D109-486D-B1CD-67D7341DF12D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="6400800" y="3314700"/>
+            <a:ext cx="685800" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="37" name="Прямоугольник: скругленные углы 36">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32EE7A35-18E7-4918-BFAA-44D9D406DE61}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6572250" y="3251200"/>
+            <a:ext cx="330200" cy="133350"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ru-RU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>232385</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>129702</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>13512</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>79308</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="38" name="Группа 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558254B4-E181-41BE-AA11-DFCCAC8F685B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1869874" y="1967149"/>
+          <a:ext cx="599872" cy="133350"/>
+          <a:chOff x="6400800" y="3251200"/>
+          <a:chExt cx="685800" cy="133350"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="39" name="Прямая соединительная линия 38">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9195026A-B4DA-42C9-AEA3-B66FF6883907}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="6400800" y="3314700"/>
+            <a:ext cx="685800" cy="0"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="none"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="40" name="Прямоугольник: скругленные углы 39">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{870725B2-DBDA-4560-A85F-AEDF51688E70}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="6572250" y="3251200"/>
+            <a:ext cx="330200" cy="133350"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ru-RU" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>72958</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>193481</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>3801</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="41" name="Прямая со стрелкой 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B26CA2A4-BE3A-4932-8635-A8B4D501A114}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1710447" y="2759971"/>
+          <a:ext cx="120523" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:headEnd type="none"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>269677</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Прямая соединительная линия 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{107F6450-97BF-4136-95E6-39C34DC1C5FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1088422" y="2058516"/>
+          <a:ext cx="3239" cy="697654"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>37325</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3239</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="Прямая соединительная линия 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{632B7386-C305-46A9-919B-65A2AA71BC17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2456234" y="2058516"/>
+          <a:ext cx="3239" cy="697654"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>70256</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>8106</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="TextBox 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BB6679E-97BD-4572-9184-80B53F43149A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="818745" y="3123660"/>
+          <a:ext cx="889000" cy="375595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>202660</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>175639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="TextBox 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB65ED84-6DBC-49AB-A7E0-9CF65ABDC359}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1840149" y="3115554"/>
+          <a:ext cx="889000" cy="375595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>16213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>32425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88665</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Блок-схема: узел 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD15A680-6E3D-4962-AB41-CD094D824B4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1052758" y="3139873"/>
+          <a:ext cx="71327" cy="72452"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>234013</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>16213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>32426</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>88665</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Блок-схема: узел 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{097D57EE-F650-4F86-A07F-4A81E2E4BD0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1325673" y="3139873"/>
+          <a:ext cx="71327" cy="72452"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>269142</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>67554</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83261</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Блок-схема: узел 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51BC104C-25E0-4BBA-A347-631246996CA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1633716" y="3134469"/>
+          <a:ext cx="71327" cy="72452"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>204291</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2703</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83261</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Блок-схема: узел 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C89EE56B-C531-4983-A5A6-27C51227C57C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1841780" y="3134469"/>
+          <a:ext cx="71327" cy="72452"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>236716</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>35128</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83261</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Блок-схема: узел 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E29B1EA-8ED2-4841-88DF-50635F5586F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2147120" y="3134469"/>
+          <a:ext cx="71327" cy="72452"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>239418</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10809</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>37830</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>83261</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Блок-схема: узел 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B1F9A96-51FA-4DD2-BA17-7CEE31DD9591}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2422737" y="3134469"/>
+          <a:ext cx="71327" cy="72452"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartConnector">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:sysClr val="window" lastClr="FFFFFF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2702</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>10808</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="55" name="Прямая соединительная линия 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA0BB609-B034-461C-8A44-8A4B5B24C86F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1913106" y="3501957"/>
+          <a:ext cx="543128" cy="172937"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>13511</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>272915</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="56" name="Прямая соединительная линия 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97612B71-28EB-48E9-90A2-24ADC55FF4D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1091660" y="3504660"/>
+          <a:ext cx="545829" cy="170234"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -7643,8 +9895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC44C08-A1D5-4906-9988-52ECBDC253C6}">
   <dimension ref="B36:AE54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AD71" sqref="AD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7754,6 +10006,82 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499C18B1-AF77-434B-B53B-6B071AD3B070}">
+  <dimension ref="D11:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D16" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+      <c r="H16" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" t="s">
+        <v>106</v>
+      </c>
+      <c r="J16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.35">
+      <c r="D17" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" t="s">
+        <v>108</v>
+      </c>
+      <c r="H17" t="s">
+        <v>108</v>
+      </c>
+      <c r="I17" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0748FA8F-6B61-4D16-A1AC-B4D429E05653}">
   <dimension ref="A1:J44"/>
   <sheetViews>
@@ -7870,7 +10198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE8F8D08-EB2F-4FE7-8856-D5C79DC74A6F}">
   <dimension ref="A1:L24"/>
   <sheetViews>

</xml_diff>